<commit_message>
latest formatted results in excel
</commit_message>
<xml_diff>
--- a/figures/COVID_deaths_by_ethnicity.xlsx
+++ b/figures/COVID_deaths_by_ethnicity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asariam/code/nhs_covid_deaths/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53924A4-40D1-3D4F-A157-01117364030B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F8012A-FB59-AD45-ADCD-40009061C13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>Deaths in Hospital from COVID-19 by ethnicity</t>
   </si>
   <si>
-    <t>Data for England up until 21st April 2020 (published 23rd April 2020)</t>
+    <t>Data for England up until 28th April 2020 (published 30th April 2020)</t>
   </si>
 </sst>
 </file>
@@ -763,9 +763,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -793,6 +790,9 @@
     <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1153,7 +1153,7 @@
   <dimension ref="C2:J41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,7 +1169,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1222,23 +1222,23 @@
       </c>
       <c r="F7" s="2">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>11354</v>
+        <v>13960</v>
       </c>
       <c r="G7" s="4">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>0.77054631828978604</v>
+        <v>0.78137243927012201</v>
       </c>
       <c r="H7" s="2">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>13487</v>
-      </c>
-      <c r="I7" s="21">
+        <v>16351</v>
+      </c>
+      <c r="I7" s="20">
         <f>F7-H7</f>
-        <v>-2133</v>
+        <v>-2391</v>
       </c>
       <c r="J7" s="3">
         <f>I7/H7</f>
-        <v>-0.15815229480240231</v>
+        <v>-0.14622958840437894</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.2">
@@ -1255,23 +1255,23 @@
       </c>
       <c r="F8" s="2">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="G8" s="4">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.09263657957244E-2</v>
+        <v>1.00750027986118E-2</v>
       </c>
       <c r="H8" s="2">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>238</v>
-      </c>
-      <c r="I8" s="35">
+        <v>289</v>
+      </c>
+      <c r="I8" s="34">
         <f t="shared" ref="I8:I34" si="0">F8-H8</f>
-        <v>-77</v>
-      </c>
-      <c r="J8" s="23">
+        <v>-109</v>
+      </c>
+      <c r="J8" s="22">
         <f t="shared" ref="J8:J34" si="1">I8/H8</f>
-        <v>-0.3235294117647059</v>
+        <v>-0.37716262975778547</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
@@ -1288,56 +1288,56 @@
       </c>
       <c r="F9" s="2">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>544</v>
+        <v>641</v>
       </c>
       <c r="G9" s="4">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.6918900576857802E-2</v>
-      </c>
-      <c r="H9" s="13">
+        <v>3.5878204410612298E-2</v>
+      </c>
+      <c r="H9" s="12">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>302</v>
-      </c>
-      <c r="I9" s="35">
+        <v>366</v>
+      </c>
+      <c r="I9" s="34">
         <f t="shared" si="0"/>
-        <v>242</v>
-      </c>
-      <c r="J9" s="23">
+        <v>275</v>
+      </c>
+      <c r="J9" s="22">
         <f t="shared" si="1"/>
-        <v>0.80132450331125826</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="24" t="s">
+        <v>0.75136612021857918</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <f>SUM(D7:D9)</f>
         <v>43023953</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <f>SUM(E7:E9)</f>
         <v>0.85573241498198405</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <f>SUM(F7:F9)</f>
-        <v>12059</v>
-      </c>
-      <c r="G10" s="27">
+        <v>14781</v>
+      </c>
+      <c r="G10" s="26">
         <f t="shared" ref="G10:I10" si="2">SUM(G7:G9)</f>
-        <v>0.81839158466236817</v>
-      </c>
-      <c r="H10" s="25">
+        <v>0.82732564647934614</v>
+      </c>
+      <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>14027</v>
-      </c>
-      <c r="I10" s="28">
+        <v>17006</v>
+      </c>
+      <c r="I10" s="27">
         <f t="shared" si="2"/>
-        <v>-1968</v>
-      </c>
-      <c r="J10" s="29">
+        <v>-2225</v>
+      </c>
+      <c r="J10" s="28">
         <f t="shared" si="1"/>
-        <v>-0.14030084836386969</v>
+        <v>-0.13083617546748205</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
@@ -1345,8 +1345,8 @@
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="21"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
@@ -1357,8 +1357,8 @@
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="21"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
@@ -1375,23 +1375,23 @@
       </c>
       <c r="F13" s="2">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>492</v>
+        <v>560</v>
       </c>
       <c r="G13" s="4">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.3389888021717003E-2</v>
-      </c>
-      <c r="H13" s="13">
+        <v>3.1344453151236899E-2</v>
+      </c>
+      <c r="H13" s="12">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>188</v>
-      </c>
-      <c r="I13" s="35">
+        <v>228</v>
+      </c>
+      <c r="I13" s="34">
         <f t="shared" si="0"/>
-        <v>304</v>
-      </c>
-      <c r="J13" s="23">
+        <v>332</v>
+      </c>
+      <c r="J13" s="22">
         <f t="shared" si="1"/>
-        <v>1.6170212765957446</v>
+        <v>1.4561403508771931</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.2">
@@ -1408,23 +1408,23 @@
       </c>
       <c r="F14" s="2">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>332</v>
+        <v>381</v>
       </c>
       <c r="G14" s="4">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.25313878520529E-2</v>
-      </c>
-      <c r="H14" s="13">
+        <v>2.1325422590395101E-2</v>
+      </c>
+      <c r="H14" s="12">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>82</v>
-      </c>
-      <c r="I14" s="35">
+        <v>100</v>
+      </c>
+      <c r="I14" s="34">
         <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="J14" s="23">
+        <v>281</v>
+      </c>
+      <c r="J14" s="22">
         <f t="shared" si="1"/>
-        <v>3.0487804878048781</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
@@ -1441,21 +1441,21 @@
       </c>
       <c r="F15" s="2">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G15" s="4">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>6.7865626060400397E-3</v>
-      </c>
-      <c r="H15" s="13">
+        <v>6.7166685324079201E-3</v>
+      </c>
+      <c r="H15" s="12">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>25</v>
-      </c>
-      <c r="I15" s="35">
+        <v>30</v>
+      </c>
+      <c r="I15" s="34">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="J15" s="23">
+        <v>90</v>
+      </c>
+      <c r="J15" s="22">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1474,23 +1474,23 @@
       </c>
       <c r="F16" s="2">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G16" s="4">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.8683406854428202E-3</v>
-      </c>
-      <c r="H16" s="13">
+        <v>3.6941676928243499E-3</v>
+      </c>
+      <c r="H16" s="12">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>36</v>
-      </c>
-      <c r="I16" s="35">
+        <v>44</v>
+      </c>
+      <c r="I16" s="34">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="J16" s="23">
+        <v>22</v>
+      </c>
+      <c r="J16" s="22">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.2">
@@ -1507,56 +1507,56 @@
       </c>
       <c r="F17" s="2">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>245</v>
+        <v>300</v>
       </c>
       <c r="G17" s="4">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.66270783847981E-2</v>
-      </c>
-      <c r="H17" s="13">
+        <v>1.6791671331019799E-2</v>
+      </c>
+      <c r="H17" s="12">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>71</v>
-      </c>
-      <c r="I17" s="35">
+        <v>87</v>
+      </c>
+      <c r="I17" s="34">
         <f t="shared" si="0"/>
-        <v>174</v>
-      </c>
-      <c r="J17" s="23">
+        <v>213</v>
+      </c>
+      <c r="J17" s="22">
         <f t="shared" si="1"/>
-        <v>2.4507042253521125</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="24" t="s">
+        <v>2.4482758620689653</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="24">
         <f>SUM(D13:D17)</f>
         <v>3898102</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="25">
         <f>SUM(E13:E17)</f>
         <v>7.7531979414027799E-2</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="24">
         <f>SUM(F13:F17)</f>
-        <v>1226</v>
-      </c>
-      <c r="G18" s="26">
+        <v>1427</v>
+      </c>
+      <c r="G18" s="25">
         <f>SUM(G13:G17)</f>
-        <v>8.3203257550050869E-2</v>
-      </c>
-      <c r="H18" s="25">
+        <v>7.987238329788407E-2</v>
+      </c>
+      <c r="H18" s="24">
         <f>SUM(H13:H17)</f>
-        <v>402</v>
-      </c>
-      <c r="I18" s="28">
+        <v>489</v>
+      </c>
+      <c r="I18" s="27">
         <f t="shared" si="0"/>
-        <v>824</v>
-      </c>
-      <c r="J18" s="29">
+        <v>938</v>
+      </c>
+      <c r="J18" s="28">
         <f t="shared" si="1"/>
-        <v>2.0497512437810945</v>
+        <v>1.918200408997955</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.2">
@@ -1564,8 +1564,8 @@
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="22"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.2">
@@ -1576,8 +1576,8 @@
       <c r="E20" s="4"/>
       <c r="F20" s="2"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="22"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.2">
@@ -1594,23 +1594,23 @@
       </c>
       <c r="F21" s="2">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>290</v>
+        <v>331</v>
       </c>
       <c r="G21" s="4">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.9681031557516101E-2</v>
-      </c>
-      <c r="H21" s="13">
+        <v>1.8526810701891799E-2</v>
+      </c>
+      <c r="H21" s="12">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>51</v>
-      </c>
-      <c r="I21" s="35">
+        <v>62</v>
+      </c>
+      <c r="I21" s="34">
         <f t="shared" si="0"/>
-        <v>239</v>
-      </c>
-      <c r="J21" s="23">
+        <v>269</v>
+      </c>
+      <c r="J21" s="22">
         <f t="shared" si="1"/>
-        <v>4.6862745098039218</v>
+        <v>4.338709677419355</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.2">
@@ -1627,23 +1627,23 @@
       </c>
       <c r="F22" s="2">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>460</v>
+        <v>525</v>
       </c>
       <c r="G22" s="4">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.1218187987784099E-2</v>
-      </c>
-      <c r="H22" s="13">
+        <v>2.93854248292846E-2</v>
+      </c>
+      <c r="H22" s="12">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>124</v>
-      </c>
-      <c r="I22" s="35">
+        <v>150</v>
+      </c>
+      <c r="I22" s="34">
         <f t="shared" si="0"/>
-        <v>336</v>
-      </c>
-      <c r="J22" s="23">
+        <v>375</v>
+      </c>
+      <c r="J22" s="22">
         <f t="shared" si="1"/>
-        <v>2.7096774193548385</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.2">
@@ -1660,56 +1660,56 @@
       </c>
       <c r="F23" s="2">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="G23" s="4">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>9.9083814048184504E-3</v>
-      </c>
-      <c r="H23" s="13">
+        <v>9.2913914698309601E-3</v>
+      </c>
+      <c r="H23" s="12">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>17</v>
-      </c>
-      <c r="I23" s="35">
+        <v>20</v>
+      </c>
+      <c r="I23" s="34">
         <f t="shared" si="0"/>
-        <v>129</v>
-      </c>
-      <c r="J23" s="23">
+        <v>146</v>
+      </c>
+      <c r="J23" s="22">
         <f t="shared" si="1"/>
-        <v>7.5882352941176467</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="24" t="s">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="24">
         <f>SUM(D21:D23)</f>
         <v>1722418</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="25">
         <f>SUM(E21:E23)</f>
         <v>3.4258333137088398E-2</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="24">
         <f>SUM(F21:F23)</f>
-        <v>896</v>
-      </c>
-      <c r="G24" s="26">
+        <v>1022</v>
+      </c>
+      <c r="G24" s="25">
         <f t="shared" ref="G24:H24" si="3">SUM(G21:G23)</f>
-        <v>6.0807600950118654E-2</v>
-      </c>
-      <c r="H24" s="25">
+        <v>5.7203627001007361E-2</v>
+      </c>
+      <c r="H24" s="24">
         <f t="shared" si="3"/>
-        <v>192</v>
-      </c>
-      <c r="I24" s="28">
+        <v>232</v>
+      </c>
+      <c r="I24" s="27">
         <f t="shared" si="0"/>
-        <v>704</v>
-      </c>
-      <c r="J24" s="27">
+        <v>790</v>
+      </c>
+      <c r="J24" s="26">
         <f t="shared" si="1"/>
-        <v>3.6666666666666665</v>
+        <v>3.4051724137931036</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.2">
@@ -1717,8 +1717,8 @@
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="22"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.2">
@@ -1729,8 +1729,8 @@
       <c r="E26" s="4"/>
       <c r="F26" s="2"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="22"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.2">
@@ -1747,89 +1747,89 @@
       </c>
       <c r="F27" s="2">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" s="4">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.4930437733288E-3</v>
-      </c>
-      <c r="H27" s="13">
+        <v>1.28736146871151E-3</v>
+      </c>
+      <c r="H27" s="12">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>18</v>
-      </c>
-      <c r="I27" s="35">
+        <v>22</v>
+      </c>
+      <c r="I27" s="34">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J27" s="23">
+        <v>1</v>
+      </c>
+      <c r="J27" s="22">
         <f t="shared" si="1"/>
-        <v>0.22222222222222221</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" s="2">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>372676</v>
+        <v>155898</v>
       </c>
       <c r="E28" s="4">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>7.4124042829310901E-3</v>
+        <v>3.1007604538537199E-3</v>
       </c>
       <c r="F28" s="2">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="G28" s="4">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.23956565999321E-3</v>
-      </c>
-      <c r="H28" s="13">
+        <v>7.2763909101085801E-4</v>
+      </c>
+      <c r="H28" s="12">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>24</v>
-      </c>
-      <c r="I28" s="35">
+        <v>8</v>
+      </c>
+      <c r="I28" s="34">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J28" s="23">
+        <v>5</v>
+      </c>
+      <c r="J28" s="22">
         <f t="shared" si="1"/>
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D29" s="2">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>155898</v>
+        <v>372676</v>
       </c>
       <c r="E29" s="4">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>3.1007604538537199E-3</v>
+        <v>7.4124042829310901E-3</v>
       </c>
       <c r="F29" s="2">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="G29" s="4">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>8.1438751272480399E-4</v>
-      </c>
-      <c r="H29" s="13">
+        <v>2.18291727303257E-3</v>
+      </c>
+      <c r="H29" s="12">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>6</v>
-      </c>
-      <c r="I29" s="35">
+        <v>29</v>
+      </c>
+      <c r="I29" s="34">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J29" s="23">
+        <v>10</v>
+      </c>
+      <c r="J29" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.34482758620689657</v>
       </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.2">
@@ -1846,56 +1846,56 @@
       </c>
       <c r="F30" s="2">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G30" s="4">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.2575500508992099E-3</v>
-      </c>
-      <c r="H30" s="13">
+        <v>3.07847307735363E-3</v>
+      </c>
+      <c r="H30" s="12">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>17</v>
-      </c>
-      <c r="I30" s="35">
+        <v>21</v>
+      </c>
+      <c r="I30" s="34">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="J30" s="23">
+        <v>34</v>
+      </c>
+      <c r="J30" s="22">
         <f t="shared" si="1"/>
-        <v>1.8235294117647058</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="24" t="s">
+        <v>1.6190476190476191</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="24">
         <f>SUM(D27:D30)</f>
         <v>1110913</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="25">
         <f>SUM(E27:E30)</f>
         <v>2.2095697815700029E-2</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="24">
         <f>SUM(F27:F30)</f>
-        <v>115</v>
-      </c>
-      <c r="G31" s="26">
+        <v>130</v>
+      </c>
+      <c r="G31" s="25">
         <f>SUM(G27:G30)</f>
-        <v>7.8045469969460239E-3</v>
-      </c>
-      <c r="H31" s="25">
+        <v>7.276390910108569E-3</v>
+      </c>
+      <c r="H31" s="24">
         <f>SUM(H27:H30)</f>
-        <v>65</v>
-      </c>
-      <c r="I31" s="28">
+        <v>80</v>
+      </c>
+      <c r="I31" s="27">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J31" s="27">
+      <c r="J31" s="26">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.2">
@@ -1903,8 +1903,8 @@
       <c r="E32" s="4"/>
       <c r="F32" s="2"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="22"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="21"/>
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.2">
@@ -1915,142 +1915,142 @@
       <c r="E33" s="4"/>
       <c r="F33" s="2"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="22"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="21"/>
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="14">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,2,FALSE)</f>
         <v>521958</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="15">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,3,FALSE)</f>
         <v>1.03815746511987E-2</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>439</v>
-      </c>
-      <c r="G34" s="16">
+        <v>506</v>
+      </c>
+      <c r="G34" s="15">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.9793009840515701E-2</v>
-      </c>
-      <c r="H34" s="17">
+        <v>2.8321952311653398E-2</v>
+      </c>
+      <c r="H34" s="16">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>48</v>
-      </c>
-      <c r="I34" s="35">
+        <v>59</v>
+      </c>
+      <c r="I34" s="34">
         <f t="shared" si="0"/>
-        <v>391</v>
-      </c>
-      <c r="J34" s="36">
+        <v>447</v>
+      </c>
+      <c r="J34" s="35">
         <f t="shared" si="1"/>
-        <v>8.1458333333333339</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="31" t="s">
+        <v>7.5762711864406782</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="32">
-        <f>D34</f>
+      <c r="D35" s="31">
+        <f t="shared" ref="D35:J35" si="4">D34</f>
         <v>521958</v>
       </c>
-      <c r="E35" s="33">
-        <f>E34</f>
+      <c r="E35" s="32">
+        <f t="shared" si="4"/>
         <v>1.03815746511987E-2</v>
       </c>
-      <c r="F35" s="32">
-        <f>F34</f>
-        <v>439</v>
-      </c>
-      <c r="G35" s="33">
-        <f>G34</f>
-        <v>2.9793009840515701E-2</v>
-      </c>
-      <c r="H35" s="32">
-        <f>H34</f>
-        <v>48</v>
-      </c>
-      <c r="I35" s="28">
-        <f>I34</f>
-        <v>391</v>
-      </c>
-      <c r="J35" s="34">
-        <f>J34</f>
-        <v>8.1458333333333339</v>
+      <c r="F35" s="31">
+        <f t="shared" si="4"/>
+        <v>506</v>
+      </c>
+      <c r="G35" s="32">
+        <f t="shared" si="4"/>
+        <v>2.8321952311653398E-2</v>
+      </c>
+      <c r="H35" s="31">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="I35" s="27">
+        <f t="shared" si="4"/>
+        <v>447</v>
+      </c>
+      <c r="J35" s="33">
+        <f t="shared" si="4"/>
+        <v>7.5762711864406782</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C36" s="14"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="18"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="19" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="9">
         <f>SUM(D7:D9,D13:D17,D21:D23,D27:D30,D34)</f>
         <v>50277344</v>
       </c>
-      <c r="E37" s="12">
-        <f t="shared" ref="E37:G37" si="4">SUM(E7:E9,E13:E17,E21:E23,E27:E30,E34)</f>
+      <c r="E37" s="11">
+        <f t="shared" ref="E37:G37" si="5">SUM(E7:E9,E13:E17,E21:E23,E27:E30,E34)</f>
         <v>0.99999999999999911</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" si="4"/>
-        <v>14735</v>
-      </c>
-      <c r="G37" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
+        <v>17866</v>
+      </c>
+      <c r="G37" s="11">
+        <f t="shared" si="5"/>
         <v>0.99999999999999944</v>
       </c>
       <c r="H37" s="9">
         <f>SUM(H7:H9,H13:H17,H21:H23,H27:H30,H34)+1</f>
-        <v>14735</v>
+        <v>17867</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J34">
@@ -2070,7 +2070,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2135,25 +2135,25 @@
         <v>1.54211805619644E-2</v>
       </c>
       <c r="E2">
-        <v>245</v>
+        <v>300</v>
       </c>
       <c r="F2">
-        <v>1.66270783847981E-2</v>
+        <v>1.6791671331019799E-2</v>
       </c>
       <c r="G2">
-        <v>227</v>
+        <v>276</v>
       </c>
       <c r="H2">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="I2">
-        <v>4.8426822499843102E-3</v>
+        <v>4.8490767389307299E-3</v>
       </c>
       <c r="J2">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="K2">
-        <v>3.4507042253521099</v>
+        <v>3.44827586206896</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2170,22 +2170,22 @@
         <v>7.8119082821876901E-3</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F3">
-        <v>6.7865626060400397E-3</v>
+        <v>6.7166685324079201E-3</v>
       </c>
       <c r="G3">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="H3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I3">
-        <v>1.70095940574708E-3</v>
+        <v>1.70276882896314E-3</v>
       </c>
       <c r="J3">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -2205,25 +2205,25 @@
         <v>7.3719486852766103E-3</v>
       </c>
       <c r="E4">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F4">
-        <v>3.8683406854428202E-3</v>
+        <v>3.6941676928243499E-3</v>
       </c>
       <c r="G4">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="H4">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I4">
-        <v>2.46378271492693E-3</v>
+        <v>2.4653978218215499E-3</v>
       </c>
       <c r="J4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K4">
-        <v>1.5833333333333299</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2240,25 +2240,25 @@
         <v>2.66202407191597E-2</v>
       </c>
       <c r="E5">
-        <v>492</v>
+        <v>560</v>
       </c>
       <c r="F5">
-        <v>3.3389888021717003E-2</v>
+        <v>3.1344453151236899E-2</v>
       </c>
       <c r="G5">
-        <v>392</v>
+        <v>476</v>
       </c>
       <c r="H5">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="I5">
-        <v>1.27850711963693E-2</v>
+        <v>1.2786826879925E-2</v>
       </c>
       <c r="J5">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="K5">
-        <v>2.6170212765957399</v>
+        <v>2.45614035087719</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2275,25 +2275,25 @@
         <v>2.0306701165439402E-2</v>
       </c>
       <c r="E6">
-        <v>332</v>
+        <v>381</v>
       </c>
       <c r="F6">
-        <v>2.25313878520529E-2</v>
+        <v>2.1325422590395101E-2</v>
       </c>
       <c r="G6">
-        <v>299</v>
+        <v>363</v>
       </c>
       <c r="H6">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="I6">
-        <v>5.5871139249617299E-3</v>
+        <v>5.5934417942234103E-3</v>
       </c>
       <c r="J6">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="K6">
-        <v>4.0487804878048701</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2310,25 +2310,25 @@
         <v>1.8186302760941301E-2</v>
       </c>
       <c r="E7">
-        <v>290</v>
+        <v>331</v>
       </c>
       <c r="F7">
-        <v>1.9681031557516101E-2</v>
+        <v>1.8526810701891799E-2</v>
       </c>
       <c r="G7">
-        <v>268</v>
+        <v>325</v>
       </c>
       <c r="H7">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="I7">
-        <v>3.4479649359432001E-3</v>
+        <v>3.4631259241183101E-3</v>
       </c>
       <c r="J7">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="K7">
-        <v>5.68627450980392</v>
+        <v>5.3387096774193497</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -2345,25 +2345,25 @@
         <v>5.0447175570769998E-3</v>
       </c>
       <c r="E8">
+        <v>166</v>
+      </c>
+      <c r="F8">
+        <v>9.2913914698309601E-3</v>
+      </c>
+      <c r="G8">
+        <v>90</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>1.13851580556242E-3</v>
+      </c>
+      <c r="J8">
         <v>146</v>
       </c>
-      <c r="F8">
-        <v>9.9083814048184504E-3</v>
-      </c>
-      <c r="G8">
-        <v>74</v>
-      </c>
-      <c r="H8">
-        <v>17</v>
-      </c>
-      <c r="I8">
-        <v>1.13342218834618E-3</v>
-      </c>
-      <c r="J8">
-        <v>129</v>
-      </c>
       <c r="K8">
-        <v>8.5882352941176396</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -2380,25 +2380,25 @@
         <v>1.1027312819070101E-2</v>
       </c>
       <c r="E9">
-        <v>460</v>
+        <v>525</v>
       </c>
       <c r="F9">
-        <v>3.1218187987784099E-2</v>
+        <v>2.93854248292846E-2</v>
       </c>
       <c r="G9">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="H9">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="I9">
-        <v>8.4092576724444906E-3</v>
+        <v>8.4163937098684707E-3</v>
       </c>
       <c r="J9">
-        <v>336</v>
+        <v>375</v>
       </c>
       <c r="K9">
-        <v>3.7096774193548301</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -2415,25 +2415,25 @@
         <v>5.3595711022443801E-3</v>
       </c>
       <c r="E10">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F10">
-        <v>3.2575500508992099E-3</v>
+        <v>3.07847307735363E-3</v>
       </c>
       <c r="G10">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="H10">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I10">
-        <v>1.1793532056018599E-3</v>
+        <v>1.1814125634753501E-3</v>
       </c>
       <c r="J10">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K10">
-        <v>2.8235294117646998</v>
+        <v>2.6190476190476102</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -2450,25 +2450,25 @@
         <v>6.2229619766708396E-3</v>
       </c>
       <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>1.28736146871151E-3</v>
+      </c>
+      <c r="G11">
+        <v>111</v>
+      </c>
+      <c r="H11">
         <v>22</v>
       </c>
-      <c r="F11">
-        <v>1.4930437733288E-3</v>
-      </c>
-      <c r="G11">
-        <v>92</v>
-      </c>
-      <c r="H11">
-        <v>18</v>
-      </c>
       <c r="I11">
-        <v>1.2123989030345299E-3</v>
+        <v>1.2153048101368399E-3</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>1.2222222222222201</v>
+        <v>1.0454545454545401</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -2485,25 +2485,25 @@
         <v>3.1007604538537199E-3</v>
       </c>
       <c r="E12">
-        <v>12</v>
-      </c>
-      <c r="F12" s="11">
-        <v>8.1438751272480399E-4</v>
+        <v>13</v>
+      </c>
+      <c r="F12" s="10">
+        <v>7.2763909101085801E-4</v>
       </c>
       <c r="G12">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H12">
-        <v>6</v>
-      </c>
-      <c r="I12" s="11">
-        <v>4.2888195868568302E-4</v>
+        <v>8</v>
+      </c>
+      <c r="I12" s="10">
+        <v>4.3067424107091901E-4</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -2520,25 +2520,25 @@
         <v>7.4124042829310901E-3</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F13">
-        <v>2.23956565999321E-3</v>
+        <v>2.18291727303257E-3</v>
       </c>
       <c r="G13">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="H13">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I13">
-        <v>1.6205554061244399E-3</v>
+        <v>1.6246638924235801E-3</v>
       </c>
       <c r="J13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <v>1.375</v>
+        <v>1.3448275862068899</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -2555,25 +2555,25 @@
         <v>1.03815746511987E-2</v>
       </c>
       <c r="E14">
-        <v>439</v>
+        <v>506</v>
       </c>
       <c r="F14">
-        <v>2.9793009840515701E-2</v>
+        <v>2.8321952311653398E-2</v>
       </c>
       <c r="G14">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="H14">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="I14">
-        <v>3.2859162640448999E-3</v>
+        <v>3.2906775821027298E-3</v>
       </c>
       <c r="J14">
-        <v>391</v>
+        <v>447</v>
       </c>
       <c r="K14">
-        <v>9.1458333333333304</v>
+        <v>8.5762711864406693</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2590,25 +2590,25 @@
         <v>4.8608633741671001E-2</v>
       </c>
       <c r="E15">
-        <v>544</v>
+        <v>641</v>
       </c>
       <c r="F15">
-        <v>3.6918900576857802E-2</v>
+        <v>3.5878204410612298E-2</v>
       </c>
       <c r="G15">
-        <v>716</v>
+        <v>868</v>
       </c>
       <c r="H15">
-        <v>302</v>
+        <v>366</v>
       </c>
       <c r="I15">
-        <v>2.0466997388231802E-2</v>
+        <v>2.04896456261392E-2</v>
       </c>
       <c r="J15">
-        <v>242</v>
+        <v>275</v>
       </c>
       <c r="K15">
-        <v>1.8013245033112499</v>
+        <v>1.75136612021857</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -2625,25 +2625,25 @@
         <v>0.79703406767071805</v>
       </c>
       <c r="E16">
-        <v>11354</v>
+        <v>13960</v>
       </c>
       <c r="F16">
-        <v>0.77054631828978604</v>
+        <v>0.78137243927012201</v>
       </c>
       <c r="G16">
-        <v>11744</v>
+        <v>14240</v>
       </c>
       <c r="H16">
-        <v>13487</v>
+        <v>16351</v>
       </c>
       <c r="I16">
-        <v>0.91527370252833795</v>
+        <v>0.91520340729712901</v>
       </c>
       <c r="J16">
-        <v>-2133</v>
+        <v>-2391</v>
       </c>
       <c r="K16">
-        <v>0.841847705197597</v>
+        <v>0.85377041159562095</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -2660,25 +2660,25 @@
         <v>1.0089713569595E-2</v>
       </c>
       <c r="E17">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="F17">
-        <v>1.09263657957244E-2</v>
+        <v>1.00750027986118E-2</v>
       </c>
       <c r="G17">
-        <v>149</v>
+        <v>180</v>
       </c>
       <c r="H17">
-        <v>238</v>
+        <v>289</v>
       </c>
       <c r="I17">
-        <v>1.6161940057214799E-2</v>
+        <v>1.61486664841092E-2</v>
       </c>
       <c r="J17">
-        <v>-77</v>
+        <v>-109</v>
       </c>
       <c r="K17">
-        <v>0.67647058823529405</v>
+        <v>0.62283737024221397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to include deaths to 12th May 2020 - also fixed bug in population aggregation for young ages
</commit_message>
<xml_diff>
--- a/figures/COVID_deaths_by_ethnicity.xlsx
+++ b/figures/COVID_deaths_by_ethnicity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asariam/code/nhs_covid_deaths/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F8012A-FB59-AD45-ADCD-40009061C13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721B5BB0-C10C-814A-A179-1539B5624DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="1360" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID_deaths_by_ethnicity" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
     <t>Deaths in Hospital from COVID-19 by ethnicity</t>
   </si>
   <si>
-    <t>Data for England up until 28th April 2020 (published 30th April 2020)</t>
+    <t>Data for England up until 12th May 2020 (published 14th May 2020)</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1153,10 +1153,10 @@
   <dimension ref="C2:J41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
@@ -1168,17 +1168,17 @@
     <col min="10" max="10" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" ht="21">
       <c r="C2" s="36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:10">
       <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:10" ht="47" customHeight="1">
       <c r="C5" s="6"/>
       <c r="D5" s="7" t="s">
         <v>21</v>
@@ -1202,145 +1202,145 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:10">
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:10">
       <c r="C7" t="str">
         <f>raw_data!B16</f>
         <v>British</v>
       </c>
       <c r="D7" s="2">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>40072756</v>
+        <v>42279236</v>
       </c>
       <c r="E7" s="4">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>0.79703406767071805</v>
+        <v>0.79753399842482298</v>
       </c>
       <c r="F7" s="2">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>13960</v>
+        <v>17117</v>
       </c>
       <c r="G7" s="4">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>0.78137243927012201</v>
+        <v>0.78793039955809197</v>
       </c>
       <c r="H7" s="2">
         <f>VLOOKUP($C7,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>16351</v>
+        <v>19886</v>
       </c>
       <c r="I7" s="20">
         <f>F7-H7</f>
-        <v>-2391</v>
+        <v>-2769</v>
       </c>
       <c r="J7" s="3">
         <f>I7/H7</f>
-        <v>-0.14622958840437894</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
+        <v>-0.13924368902745651</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="2">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>507284</v>
+        <v>517001</v>
       </c>
       <c r="E8" s="4">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>1.0089713569595E-2</v>
+        <v>9.7524438407456497E-3</v>
       </c>
       <c r="F8" s="2">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="G8" s="4">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.00750027986118E-2</v>
+        <v>1.0081016387405601E-2</v>
       </c>
       <c r="H8" s="2">
         <f>VLOOKUP($C8,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>289</v>
+        <v>351</v>
       </c>
       <c r="I8" s="34">
         <f t="shared" ref="I8:I34" si="0">F8-H8</f>
-        <v>-109</v>
+        <v>-132</v>
       </c>
       <c r="J8" s="22">
         <f t="shared" ref="J8:J34" si="1">I8/H8</f>
-        <v>-0.37716262975778547</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
+        <v>-0.37606837606837606</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>2443913</v>
+        <v>2484905</v>
       </c>
       <c r="E9" s="4">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>4.8608633741671001E-2</v>
+        <v>4.6873983729408798E-2</v>
       </c>
       <c r="F9" s="2">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>641</v>
+        <v>751</v>
       </c>
       <c r="G9" s="4">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.5878204410612298E-2</v>
+        <v>3.4570060762290501E-2</v>
       </c>
       <c r="H9" s="12">
         <f>VLOOKUP($C9,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>366</v>
+        <v>445</v>
       </c>
       <c r="I9" s="34">
         <f t="shared" si="0"/>
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="J9" s="22">
         <f t="shared" si="1"/>
-        <v>0.75136612021857918</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" s="29" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.68764044943820224</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" s="29" customFormat="1">
       <c r="C10" s="23" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="24">
         <f>SUM(D7:D9)</f>
-        <v>43023953</v>
+        <v>45281142</v>
       </c>
       <c r="E10" s="25">
         <f>SUM(E7:E9)</f>
-        <v>0.85573241498198405</v>
+        <v>0.85416042599497743</v>
       </c>
       <c r="F10" s="24">
         <f>SUM(F7:F9)</f>
-        <v>14781</v>
+        <v>18087</v>
       </c>
       <c r="G10" s="26">
         <f t="shared" ref="G10:I10" si="2">SUM(G7:G9)</f>
-        <v>0.82732564647934614</v>
+        <v>0.83258147670778804</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>17006</v>
+        <v>20682</v>
       </c>
       <c r="I10" s="27">
         <f t="shared" si="2"/>
-        <v>-2225</v>
+        <v>-2595</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" si="1"/>
-        <v>-0.13083617546748205</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+        <v>-0.12547142442703801</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
       <c r="D11" s="2"/>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
@@ -1349,7 +1349,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:10">
       <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1361,205 +1361,205 @@
       <c r="I12" s="20"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:10">
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="2">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>1338395</v>
+        <v>1395702</v>
       </c>
       <c r="E13" s="4">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>2.66202407191597E-2</v>
+        <v>2.6327812467318999E-2</v>
       </c>
       <c r="F13" s="2">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>560</v>
+        <v>665</v>
       </c>
       <c r="G13" s="4">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.1344453151236899E-2</v>
+        <v>3.06113054686061E-2</v>
       </c>
       <c r="H13" s="12">
         <f>VLOOKUP($C13,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>228</v>
+        <v>277</v>
       </c>
       <c r="I13" s="34">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>388</v>
       </c>
       <c r="J13" s="22">
         <f t="shared" si="1"/>
-        <v>1.4561403508771931</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+        <v>1.4007220216606497</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10">
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>1020967</v>
+        <v>1112282</v>
       </c>
       <c r="E14" s="4">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>2.0306701165439402E-2</v>
+        <v>2.0981521776693299E-2</v>
       </c>
       <c r="F14" s="2">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>381</v>
+        <v>448</v>
       </c>
       <c r="G14" s="4">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.1325422590395101E-2</v>
+        <v>2.0622353157797799E-2</v>
       </c>
       <c r="H14" s="12">
         <f>VLOOKUP($C14,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="I14" s="34">
         <f t="shared" si="0"/>
-        <v>281</v>
+        <v>327</v>
       </c>
       <c r="J14" s="22">
         <f t="shared" si="1"/>
-        <v>2.81</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
+        <v>2.7024793388429753</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>392762</v>
+        <v>436514</v>
       </c>
       <c r="E15" s="4">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>7.8119082821876901E-3</v>
+        <v>8.2341780203505303E-3</v>
       </c>
       <c r="F15" s="2">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="G15" s="4">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>6.7166685324079201E-3</v>
+        <v>6.7206775916037499E-3</v>
       </c>
       <c r="H15" s="12">
         <f>VLOOKUP($C15,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I15" s="34">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="J15" s="22">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+        <v>2.9459459459459461</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="2">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>370642</v>
+        <v>379503</v>
       </c>
       <c r="E16" s="4">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>7.3719486852766103E-3</v>
+        <v>7.1587515205860297E-3</v>
       </c>
       <c r="F16" s="2">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G16" s="4">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.6941676928243499E-3</v>
+        <v>3.5904989872951498E-3</v>
       </c>
       <c r="H16" s="12">
         <f>VLOOKUP($C16,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I16" s="34">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J16" s="22">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+        <v>0.47169811320754718</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10">
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>775336</v>
+        <v>819402</v>
       </c>
       <c r="E17" s="4">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>1.54211805619644E-2</v>
+        <v>1.54567824588243E-2</v>
       </c>
       <c r="F17" s="2">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>300</v>
+        <v>366</v>
       </c>
       <c r="G17" s="4">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.6791671331019799E-2</v>
+        <v>1.6847726017307999E-2</v>
       </c>
       <c r="H17" s="12">
         <f>VLOOKUP($C17,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="I17" s="34">
         <f t="shared" si="0"/>
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="J17" s="22">
         <f t="shared" si="1"/>
-        <v>2.4482758620689653</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" s="29" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2.4857142857142858</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" s="29" customFormat="1">
       <c r="C18" s="23" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="24">
         <f>SUM(D13:D17)</f>
-        <v>3898102</v>
+        <v>4143403</v>
       </c>
       <c r="E18" s="25">
         <f>SUM(E13:E17)</f>
-        <v>7.7531979414027799E-2</v>
+        <v>7.815904624377315E-2</v>
       </c>
       <c r="F18" s="24">
         <f>SUM(F13:F17)</f>
-        <v>1427</v>
+        <v>1703</v>
       </c>
       <c r="G18" s="25">
         <f>SUM(G13:G17)</f>
-        <v>7.987238329788407E-2</v>
+        <v>7.8392561222610804E-2</v>
       </c>
       <c r="H18" s="24">
         <f>SUM(H13:H17)</f>
-        <v>489</v>
+        <v>593</v>
       </c>
       <c r="I18" s="27">
         <f t="shared" si="0"/>
-        <v>938</v>
+        <v>1110</v>
       </c>
       <c r="J18" s="28">
         <f t="shared" si="1"/>
-        <v>1.918200408997955</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+        <v>1.8718381112984823</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10">
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
@@ -1568,7 +1568,7 @@
       <c r="I19" s="21"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:10">
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1580,139 +1580,139 @@
       <c r="I20" s="21"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:10">
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="2">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>914359</v>
+        <v>977741</v>
       </c>
       <c r="E21" s="4">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>1.8186302760941301E-2</v>
+        <v>1.8443608800165701E-2</v>
       </c>
       <c r="F21" s="2">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>331</v>
+        <v>394</v>
       </c>
       <c r="G21" s="4">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.8526810701891799E-2</v>
+        <v>1.8136623089670401E-2</v>
       </c>
       <c r="H21" s="12">
         <f>VLOOKUP($C21,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="I21" s="34">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>319</v>
       </c>
       <c r="J21" s="22">
         <f t="shared" si="1"/>
-        <v>4.338709677419355</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+        <v>4.253333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10">
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="2">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>554424</v>
+        <v>591016</v>
       </c>
       <c r="E22" s="4">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>1.1027312819070101E-2</v>
+        <v>1.1148625145758101E-2</v>
       </c>
       <c r="F22" s="2">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>525</v>
+        <v>601</v>
       </c>
       <c r="G22" s="4">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.93854248292846E-2</v>
+        <v>2.7665255017492101E-2</v>
       </c>
       <c r="H22" s="12">
         <f>VLOOKUP($C22,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>150</v>
+        <v>183</v>
       </c>
       <c r="I22" s="34">
         <f t="shared" si="0"/>
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="J22" s="22">
         <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+        <v>2.2841530054644807</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10">
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="2">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>253635</v>
+        <v>277857</v>
       </c>
       <c r="E23" s="4">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>5.0447175570769998E-3</v>
+        <v>5.2413530887910498E-3</v>
       </c>
       <c r="F23" s="2">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="G23" s="4">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>9.2913914698309601E-3</v>
+        <v>9.1603756214325097E-3</v>
       </c>
       <c r="H23" s="12">
         <f>VLOOKUP($C23,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I23" s="34">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="J23" s="22">
         <f t="shared" si="1"/>
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" s="23" customFormat="1">
       <c r="C24" s="23" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="24">
         <f>SUM(D21:D23)</f>
-        <v>1722418</v>
+        <v>1846614</v>
       </c>
       <c r="E24" s="25">
         <f>SUM(E21:E23)</f>
-        <v>3.4258333137088398E-2</v>
+        <v>3.4833587034714848E-2</v>
       </c>
       <c r="F24" s="24">
         <f>SUM(F21:F23)</f>
-        <v>1022</v>
+        <v>1194</v>
       </c>
       <c r="G24" s="25">
         <f t="shared" ref="G24:H24" si="3">SUM(G21:G23)</f>
-        <v>5.7203627001007361E-2</v>
+        <v>5.4962253728595013E-2</v>
       </c>
       <c r="H24" s="24">
         <f t="shared" si="3"/>
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="I24" s="27">
         <f t="shared" si="0"/>
-        <v>790</v>
+        <v>911</v>
       </c>
       <c r="J24" s="26">
         <f t="shared" si="1"/>
-        <v>3.4051724137931036</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+        <v>3.2190812720848054</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10">
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
@@ -1721,7 +1721,7 @@
       <c r="I25" s="21"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:10">
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1733,62 +1733,62 @@
       <c r="I26" s="21"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:10">
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="2">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>312874</v>
+        <v>332708</v>
       </c>
       <c r="E27" s="4">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>6.2229619766708396E-3</v>
+        <v>6.2760344474513596E-3</v>
       </c>
       <c r="F27" s="2">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G27" s="4">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>1.28736146871151E-3</v>
+        <v>1.28889707236236E-3</v>
       </c>
       <c r="H27" s="12">
         <f>VLOOKUP($C27,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I27" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" s="22">
         <f t="shared" si="1"/>
-        <v>4.5454545454545456E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>155898</v>
+        <v>161550</v>
       </c>
       <c r="E28" s="4">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>3.1007604538537199E-3</v>
+        <v>3.0473970117513502E-3</v>
       </c>
       <c r="F28" s="2">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G28" s="4">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>7.2763909101085801E-4</v>
+        <v>6.4444853618118197E-4</v>
       </c>
       <c r="H28" s="12">
         <f>VLOOKUP($C28,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I28" s="34">
         <f t="shared" si="0"/>
@@ -1796,109 +1796,109 @@
       </c>
       <c r="J28" s="22">
         <f t="shared" si="1"/>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="2">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>372676</v>
+        <v>415616</v>
       </c>
       <c r="E29" s="4">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>7.4124042829310901E-3</v>
+        <v>7.8399687801674299E-3</v>
       </c>
       <c r="F29" s="2">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G29" s="4">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.18291727303257E-3</v>
+        <v>2.02540968514085E-3</v>
       </c>
       <c r="H29" s="12">
         <f>VLOOKUP($C29,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I29" s="34">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J29" s="22">
         <f t="shared" si="1"/>
-        <v>0.34482758620689657</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="2">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>269465</v>
+        <v>283005</v>
       </c>
       <c r="E30" s="4">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>5.3595711022443801E-3</v>
+        <v>5.3384623417560501E-3</v>
       </c>
       <c r="F30" s="2">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="G30" s="4">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>3.07847307735363E-3</v>
+        <v>3.17621064260725E-3</v>
       </c>
       <c r="H30" s="12">
         <f>VLOOKUP($C30,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I30" s="34">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J30" s="22">
         <f t="shared" si="1"/>
-        <v>1.6190476190476191</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1.6538461538461537</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" s="23" customFormat="1">
       <c r="C31" s="23" t="s">
         <v>46</v>
       </c>
       <c r="D31" s="24">
         <f>SUM(D27:D30)</f>
-        <v>1110913</v>
+        <v>1192879</v>
       </c>
       <c r="E31" s="25">
         <f>SUM(E27:E30)</f>
-        <v>2.2095697815700029E-2</v>
+        <v>2.250186258112619E-2</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F27:F30)</f>
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="G31" s="25">
         <f>SUM(G27:G30)</f>
-        <v>7.276390910108569E-3</v>
+        <v>7.1349659362916424E-3</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H27:H30)</f>
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="I31" s="27">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="J31" s="26">
         <f t="shared" si="1"/>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+        <v>0.61458333333333337</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
       <c r="D32" s="2"/>
       <c r="E32" s="4"/>
       <c r="F32" s="2"/>
@@ -1907,7 +1907,7 @@
       <c r="I32" s="21"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:10">
       <c r="C33" s="1" t="s">
         <v>20</v>
       </c>
@@ -1919,73 +1919,73 @@
       <c r="I33" s="21"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10">
       <c r="C34" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="14">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,2,FALSE)</f>
-        <v>521958</v>
+        <v>548418</v>
       </c>
       <c r="E34" s="15">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,3,FALSE)</f>
-        <v>1.03815746511987E-2</v>
+        <v>1.03450781454079E-2</v>
       </c>
       <c r="F34" s="14">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,4,FALSE)</f>
-        <v>506</v>
+        <v>585</v>
       </c>
       <c r="G34" s="15">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,5,FALSE)</f>
-        <v>2.8321952311653398E-2</v>
+        <v>2.6928742404713601E-2</v>
       </c>
       <c r="H34" s="16">
         <f>VLOOKUP($C34,raw_data!$B$2:$K$17,7,FALSE)</f>
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="I34" s="34">
         <f t="shared" si="0"/>
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="J34" s="35">
         <f t="shared" si="1"/>
-        <v>7.5762711864406782</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>7.23943661971831</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" s="23" customFormat="1">
       <c r="C35" s="30" t="s">
         <v>47</v>
       </c>
       <c r="D35" s="31">
         <f t="shared" ref="D35:J35" si="4">D34</f>
-        <v>521958</v>
+        <v>548418</v>
       </c>
       <c r="E35" s="32">
         <f t="shared" si="4"/>
-        <v>1.03815746511987E-2</v>
+        <v>1.03450781454079E-2</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="4"/>
-        <v>506</v>
+        <v>585</v>
       </c>
       <c r="G35" s="32">
         <f t="shared" si="4"/>
-        <v>2.8321952311653398E-2</v>
+        <v>2.6928742404713601E-2</v>
       </c>
       <c r="H35" s="31">
         <f t="shared" si="4"/>
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="I35" s="27">
         <f t="shared" si="4"/>
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="J35" s="33">
         <f t="shared" si="4"/>
-        <v>7.5762711864406782</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+        <v>7.23943661971831</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10">
       <c r="C36" s="13"/>
       <c r="D36" s="14"/>
       <c r="E36" s="15"/>
@@ -1995,34 +1995,34 @@
       <c r="I36" s="17"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10">
       <c r="C37" s="19" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="9">
         <f>SUM(D7:D9,D13:D17,D21:D23,D27:D30,D34)</f>
-        <v>50277344</v>
+        <v>53012456</v>
       </c>
       <c r="E37" s="11">
         <f t="shared" ref="E37:G37" si="5">SUM(E7:E9,E13:E17,E21:E23,E27:E30,E34)</f>
-        <v>0.99999999999999911</v>
+        <v>0.99999999999999956</v>
       </c>
       <c r="F37" s="9">
         <f t="shared" si="5"/>
-        <v>17866</v>
+        <v>21724</v>
       </c>
       <c r="G37" s="11">
         <f t="shared" si="5"/>
-        <v>0.99999999999999944</v>
+        <v>0.99999999999999889</v>
       </c>
       <c r="H37" s="9">
         <f>SUM(H7:H9,H13:H17,H21:H23,H27:H30,H34)+1</f>
-        <v>17867</v>
+        <v>21726</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10">
       <c r="E39" s="37" t="s">
         <v>28</v>
       </c>
@@ -2032,7 +2032,7 @@
       <c r="I39" s="37"/>
       <c r="J39" s="37"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:10">
       <c r="E40" s="37" t="s">
         <v>29</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="I40" s="37"/>
       <c r="J40" s="37"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:10">
       <c r="E41" s="37" t="s">
         <v>30</v>
       </c>
@@ -2073,7 +2073,7 @@
       <selection sqref="A1:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
@@ -2086,7 +2086,7 @@
     <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2129,34 +2129,34 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>775336</v>
+        <v>819402</v>
       </c>
       <c r="D2">
-        <v>1.54211805619644E-2</v>
+        <v>1.54567824588243E-2</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>366</v>
       </c>
       <c r="F2">
-        <v>1.6791671331019799E-2</v>
+        <v>1.6847726017307999E-2</v>
       </c>
       <c r="G2">
-        <v>276</v>
+        <v>336</v>
       </c>
       <c r="H2">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="I2">
-        <v>4.8490767389307299E-3</v>
+        <v>4.8257658015763401E-3</v>
       </c>
       <c r="J2">
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="K2">
-        <v>3.44827586206896</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.48571428571428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -2164,34 +2164,34 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>392762</v>
+        <v>436514</v>
       </c>
       <c r="D3">
-        <v>7.8119082821876901E-3</v>
+        <v>8.2341780203505303E-3</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="F3">
-        <v>6.7166685324079201E-3</v>
+        <v>6.7206775916037499E-3</v>
       </c>
       <c r="G3">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="H3">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I3">
-        <v>1.70276882896314E-3</v>
+        <v>1.69538747266972E-3</v>
       </c>
       <c r="J3">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="K3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.9459459459459398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2199,34 +2199,34 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>370642</v>
+        <v>379503</v>
       </c>
       <c r="D4">
-        <v>7.3719486852766103E-3</v>
+        <v>7.1587515205860297E-3</v>
       </c>
       <c r="E4">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F4">
-        <v>3.6941676928243499E-3</v>
+        <v>3.5904989872951498E-3</v>
       </c>
       <c r="G4">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="H4">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I4">
-        <v>2.4653978218215499E-3</v>
+        <v>2.45594583315349E-3</v>
       </c>
       <c r="J4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.47169811320754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2234,34 +2234,34 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1338395</v>
+        <v>1395702</v>
       </c>
       <c r="D5">
-        <v>2.66202407191597E-2</v>
+        <v>2.6327812467318999E-2</v>
       </c>
       <c r="E5">
-        <v>560</v>
+        <v>665</v>
       </c>
       <c r="F5">
-        <v>3.1344453151236899E-2</v>
+        <v>3.06113054686061E-2</v>
       </c>
       <c r="G5">
-        <v>476</v>
+        <v>572</v>
       </c>
       <c r="H5">
-        <v>228</v>
+        <v>277</v>
       </c>
       <c r="I5">
-        <v>1.2786826879925E-2</v>
+        <v>1.2745207923964399E-2</v>
       </c>
       <c r="J5">
-        <v>332</v>
+        <v>388</v>
       </c>
       <c r="K5">
-        <v>2.45614035087719</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2.40072202166064</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2269,34 +2269,34 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>1020967</v>
+        <v>1112282</v>
       </c>
       <c r="D6">
-        <v>2.0306701165439402E-2</v>
+        <v>2.0981521776693299E-2</v>
       </c>
       <c r="E6">
-        <v>381</v>
+        <v>448</v>
       </c>
       <c r="F6">
-        <v>2.1325422590395101E-2</v>
+        <v>2.0622353157797799E-2</v>
       </c>
       <c r="G6">
-        <v>363</v>
+        <v>456</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="I6">
-        <v>5.5934417942234103E-3</v>
+        <v>5.5731356410174803E-3</v>
       </c>
       <c r="J6">
-        <v>281</v>
+        <v>327</v>
       </c>
       <c r="K6">
-        <v>3.81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.70247933884297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2304,34 +2304,34 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>914359</v>
+        <v>977741</v>
       </c>
       <c r="D7">
-        <v>1.8186302760941301E-2</v>
+        <v>1.8443608800165701E-2</v>
       </c>
       <c r="E7">
-        <v>331</v>
+        <v>394</v>
       </c>
       <c r="F7">
-        <v>1.8526810701891799E-2</v>
+        <v>1.8136623089670401E-2</v>
       </c>
       <c r="G7">
-        <v>325</v>
+        <v>401</v>
       </c>
       <c r="H7">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="I7">
-        <v>3.4631259241183101E-3</v>
+        <v>3.4401856851248901E-3</v>
       </c>
       <c r="J7">
-        <v>269</v>
+        <v>319</v>
       </c>
       <c r="K7">
-        <v>5.3387096774193497</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5.2533333333333303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -2339,34 +2339,34 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>253635</v>
+        <v>277857</v>
       </c>
       <c r="D8">
-        <v>5.0447175570769998E-3</v>
+        <v>5.2413530887910498E-3</v>
       </c>
       <c r="E8">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="F8">
-        <v>9.2913914698309601E-3</v>
+        <v>9.1603756214325097E-3</v>
       </c>
       <c r="G8">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="H8">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I8">
-        <v>1.13851580556242E-3</v>
+        <v>1.1331290452152201E-3</v>
       </c>
       <c r="J8">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="K8">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>7.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2374,34 +2374,34 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>554424</v>
+        <v>591016</v>
       </c>
       <c r="D9">
-        <v>1.1027312819070101E-2</v>
+        <v>1.1148625145758101E-2</v>
       </c>
       <c r="E9">
-        <v>525</v>
+        <v>601</v>
       </c>
       <c r="F9">
-        <v>2.93854248292846E-2</v>
+        <v>2.7665255017492101E-2</v>
       </c>
       <c r="G9">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="H9">
-        <v>150</v>
+        <v>183</v>
       </c>
       <c r="I9">
-        <v>8.4163937098684707E-3</v>
+        <v>8.4047637644137797E-3</v>
       </c>
       <c r="J9">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="K9">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.2841530054644799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2409,34 +2409,34 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>269465</v>
+        <v>283005</v>
       </c>
       <c r="D10">
-        <v>5.3595711022443801E-3</v>
+        <v>5.3384623417560501E-3</v>
       </c>
       <c r="E10">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>3.07847307735363E-3</v>
+        <v>3.17621064260725E-3</v>
       </c>
       <c r="G10">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="H10">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I10">
-        <v>1.1814125634753501E-3</v>
+        <v>1.1771409134594701E-3</v>
       </c>
       <c r="J10">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K10">
-        <v>2.6190476190476102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>2.6538461538461502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -2444,34 +2444,34 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>312874</v>
+        <v>332708</v>
       </c>
       <c r="D11">
-        <v>6.2229619766708396E-3</v>
+        <v>6.2760344474513596E-3</v>
       </c>
       <c r="E11">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F11">
-        <v>1.28736146871151E-3</v>
+        <v>1.28889707236236E-3</v>
       </c>
       <c r="G11">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="H11">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I11">
-        <v>1.2153048101368399E-3</v>
+        <v>1.21156151643394E-3</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11">
-        <v>1.0454545454545401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.07692307692307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2479,34 +2479,34 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>155898</v>
+        <v>161550</v>
       </c>
       <c r="D12">
-        <v>3.1007604538537199E-3</v>
+        <v>3.0473970117513502E-3</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" s="10">
-        <v>7.2763909101085801E-4</v>
+        <v>6.4444853618118197E-4</v>
       </c>
       <c r="G12">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I12" s="10">
-        <v>4.3067424107091901E-4</v>
+        <v>4.2803486107711102E-4</v>
       </c>
       <c r="J12">
         <v>5</v>
       </c>
       <c r="K12">
-        <v>1.625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.55555555555555</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2514,34 +2514,34 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>372676</v>
+        <v>415616</v>
       </c>
       <c r="D13">
-        <v>7.4124042829310901E-3</v>
+        <v>7.8399687801674299E-3</v>
       </c>
       <c r="E13">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F13">
-        <v>2.18291727303257E-3</v>
+        <v>2.02540968514085E-3</v>
       </c>
       <c r="G13">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="H13">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I13">
-        <v>1.6246638924235801E-3</v>
+        <v>1.6223946394365899E-3</v>
       </c>
       <c r="J13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K13">
-        <v>1.3448275862068899</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.25714285714285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2549,34 +2549,34 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>521958</v>
+        <v>548418</v>
       </c>
       <c r="D14">
-        <v>1.03815746511987E-2</v>
+        <v>1.03450781454079E-2</v>
       </c>
       <c r="E14">
-        <v>506</v>
+        <v>585</v>
       </c>
       <c r="F14">
-        <v>2.8321952311653398E-2</v>
+        <v>2.6928742404713601E-2</v>
       </c>
       <c r="G14">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="H14">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="I14">
-        <v>3.2906775821027298E-3</v>
+        <v>3.27860075308354E-3</v>
       </c>
       <c r="J14">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="K14">
-        <v>8.5762711864406693</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>8.23943661971831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2584,34 +2584,34 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>2443913</v>
+        <v>2484905</v>
       </c>
       <c r="D15">
-        <v>4.8608633741671001E-2</v>
+        <v>4.6873983729408798E-2</v>
       </c>
       <c r="E15">
-        <v>641</v>
+        <v>751</v>
       </c>
       <c r="F15">
-        <v>3.5878204410612298E-2</v>
+        <v>3.4570060762290501E-2</v>
       </c>
       <c r="G15">
-        <v>868</v>
+        <v>1018</v>
       </c>
       <c r="H15">
-        <v>366</v>
+        <v>445</v>
       </c>
       <c r="I15">
-        <v>2.04896456261392E-2</v>
+        <v>2.04696536462134E-2</v>
       </c>
       <c r="J15">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="K15">
-        <v>1.75136612021857</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.6876404494382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2619,34 +2619,34 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>40072756</v>
+        <v>42279236</v>
       </c>
       <c r="D16">
-        <v>0.79703406767071805</v>
+        <v>0.79753399842482298</v>
       </c>
       <c r="E16">
-        <v>13960</v>
+        <v>17117</v>
       </c>
       <c r="F16">
-        <v>0.78137243927012201</v>
+        <v>0.78793039955809197</v>
       </c>
       <c r="G16">
-        <v>14240</v>
+        <v>17326</v>
       </c>
       <c r="H16">
-        <v>16351</v>
+        <v>19886</v>
       </c>
       <c r="I16">
-        <v>0.91520340729712901</v>
+        <v>0.91539385264806705</v>
       </c>
       <c r="J16">
-        <v>-2391</v>
+        <v>-2769</v>
       </c>
       <c r="K16">
-        <v>0.85377041159562095</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.86075631097254302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2654,31 +2654,31 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>507284</v>
+        <v>517001</v>
       </c>
       <c r="D17">
-        <v>1.0089713569595E-2</v>
+        <v>9.7524438407456497E-3</v>
       </c>
       <c r="E17">
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="F17">
-        <v>1.00750027986118E-2</v>
+        <v>1.0081016387405601E-2</v>
       </c>
       <c r="G17">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="H17">
-        <v>289</v>
+        <v>351</v>
       </c>
       <c r="I17">
-        <v>1.61486664841092E-2</v>
+        <v>1.61452398550926E-2</v>
       </c>
       <c r="J17">
-        <v>-109</v>
+        <v>-132</v>
       </c>
       <c r="K17">
-        <v>0.62283737024221397</v>
+        <v>0.62393162393162305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>